<commit_message>
add StatTools for Respondus
</commit_message>
<xml_diff>
--- a/newman/excel/Statistics Tools copy with equation editor.xlsx
+++ b/newman/excel/Statistics Tools copy with equation editor.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan.Newman\Dropbox\github\SanJacMath.github.io\SanJacMath.github.io\newman\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FDEF52A-1647-4F57-AAA1-6CBA28137623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1BAFA81-B2C1-4E28-B7F6-45DE60381307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="ipxpIMjTBGbIwgchkjpUcV2UIfyAnwI8GfJTVRwR611cSc8NPYVaWUlZG5plp4k+StFdRfPRQ8bUjciBYwQIZQ==" workbookSaltValue="DcHgB4GQAPoChTNbbK9nyA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="975" yWindow="1620" windowWidth="22455" windowHeight="11295" tabRatio="769" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11295" tabRatio="769" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SampleStats" sheetId="1" r:id="rId1"/>
@@ -8334,9 +8334,7 @@
         <f>IF(H4&lt;&gt;"","",_xlfn.F.DIST.RT(K6,H6,H7))</f>
         <v/>
       </c>
-      <c r="N6" s="43">
-        <v>0.05</v>
-      </c>
+      <c r="N6" s="43"/>
       <c r="O6" s="23" t="str">
         <f>IF(H4&lt;&gt;"","",IF(ISBLANK(N6),"",IF(OR(NOT(ISNUMBER(N6)),N6&gt;=1,N6&lt;=0),"",_xlfn.F.INV.RT(N6,H6,H7))))</f>
         <v/>

</xml_diff>